<commit_message>
updates to drafts and tables
</commit_message>
<xml_diff>
--- a/ms/final model output and tables/Secondary model output 22-06-20.xlsx
+++ b/ms/final model output and tables/Secondary model output 22-06-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/final model output and tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7763D4A9-E645-484A-A322-FC6A1A406147}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA5BCD4-8AD2-CE4E-800E-4DC987900C08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="38300" windowHeight="19820" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19820" activeTab="5" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
   </bookViews>
   <sheets>
     <sheet name="MLMR mod 3 - Mating system" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Secondary mods 2 - Population" sheetId="2" r:id="rId3"/>
     <sheet name="Secondary mods 3 - Environment" sheetId="3" r:id="rId4"/>
     <sheet name="Secondary mods 4 - Study type" sheetId="4" r:id="rId5"/>
+    <sheet name="Publication Bias" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="268">
   <si>
     <t>Secondary model to see if age of animals in study moderates sex differences in personalities (adult vs juvenile)</t>
   </si>
@@ -611,6 +612,228 @@
   </si>
   <si>
     <t>* intercept is experimental studies</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>p=0.22</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Aggression</t>
+  </si>
+  <si>
+    <t>Boldness</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>Sociality</t>
+  </si>
+  <si>
+    <t>p=0.34</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Publication Bias: Random Effects Multilevel Models - Personality traits and taxonomic group and Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Included precision as a moderator to look for an effect of many, low sample size studies driving significant effects in our meta-analysis. </t>
+  </si>
+  <si>
+    <t>p=0.005</t>
+  </si>
+  <si>
+    <t>-0.59, 0.11</t>
+  </si>
+  <si>
+    <t>-0.59, 0.13</t>
+  </si>
+  <si>
+    <t>-0.62, 0.02</t>
+  </si>
+  <si>
+    <t>-0.36, 0.30</t>
+  </si>
+  <si>
+    <t>-1.30, 0.28</t>
+  </si>
+  <si>
+    <t>-0.02, 0.07</t>
+  </si>
+  <si>
+    <t>-0.79, 0.33</t>
+  </si>
+  <si>
+    <t>-0.63, 0.41</t>
+  </si>
+  <si>
+    <t>-0.76, 0.31</t>
+  </si>
+  <si>
+    <t>-0.64, 0.42</t>
+  </si>
+  <si>
+    <t>-1.03, 0.09</t>
+  </si>
+  <si>
+    <t>-0.05, 0.08</t>
+  </si>
+  <si>
+    <t>p=0.001</t>
+  </si>
+  <si>
+    <t>0.00, 0.73</t>
+  </si>
+  <si>
+    <t>0.27, 1.26</t>
+  </si>
+  <si>
+    <t>0.26, 0.99</t>
+  </si>
+  <si>
+    <t>-0.05, 0.80</t>
+  </si>
+  <si>
+    <t>0.02, 1.22</t>
+  </si>
+  <si>
+    <t>-0.11, -0.02</t>
+  </si>
+  <si>
+    <t>p=0.21</t>
+  </si>
+  <si>
+    <t>-0.46, 0.38</t>
+  </si>
+  <si>
+    <t>-0.17, 0.65</t>
+  </si>
+  <si>
+    <t>-0.10, 0.66</t>
+  </si>
+  <si>
+    <t>-0.21, 0.57</t>
+  </si>
+  <si>
+    <t>-0.19, 0.64</t>
+  </si>
+  <si>
+    <t>-0.09, 0.03</t>
+  </si>
+  <si>
+    <t>-0.43, 1.74</t>
+  </si>
+  <si>
+    <t>-0.51, 2.11</t>
+  </si>
+  <si>
+    <t>-0.19, 1.76</t>
+  </si>
+  <si>
+    <t>-0.06, 1.79</t>
+  </si>
+  <si>
+    <t>-0.45, 1.66</t>
+  </si>
+  <si>
+    <t>-0.56, 0.10</t>
+  </si>
+  <si>
+    <t>-0.40, 0.35</t>
+  </si>
+  <si>
+    <t>-0.56, 0.30</t>
+  </si>
+  <si>
+    <t>-0.40, 0.25</t>
+  </si>
+  <si>
+    <t>-0.67, 0.02</t>
+  </si>
+  <si>
+    <t>-0.48, 0.64</t>
+  </si>
+  <si>
+    <t>-0.04, 0.07</t>
+  </si>
+  <si>
+    <t>-0.23, 0.22</t>
+  </si>
+  <si>
+    <t>-0.30, 0.09</t>
+  </si>
+  <si>
+    <t>-0.19, 0.20</t>
+  </si>
+  <si>
+    <t>-0.16, 0.34</t>
+  </si>
+  <si>
+    <t>-0.06, 0.04</t>
+  </si>
+  <si>
+    <t>-0.21, 0.07</t>
+  </si>
+  <si>
+    <t>-0.22, 0.23</t>
+  </si>
+  <si>
+    <t>-0.17, 0.11</t>
+  </si>
+  <si>
+    <t>-0.14, 0.23</t>
+  </si>
+  <si>
+    <t>-0.11, 0.55</t>
+  </si>
+  <si>
+    <t>-0.02, 0.02</t>
+  </si>
+  <si>
+    <t>p=0.97</t>
+  </si>
+  <si>
+    <t>-0.20, 0.48</t>
+  </si>
+  <si>
+    <t>-0.21, 0.49</t>
+  </si>
+  <si>
+    <t>-0.23, 0.41</t>
+  </si>
+  <si>
+    <t>-0.25, 0.41</t>
+  </si>
+  <si>
+    <t>-0.25, 0.44</t>
+  </si>
+  <si>
+    <t>-0.04, 0.03</t>
+  </si>
+  <si>
+    <t>-0.53, 1.87</t>
+  </si>
+  <si>
+    <t>-0.15, 2.74</t>
+  </si>
+  <si>
+    <t>-0.26, 1.87</t>
+  </si>
+  <si>
+    <t>-0.45, 1.58</t>
+  </si>
+  <si>
+    <t>-0.62, 1.55</t>
+  </si>
+  <si>
+    <t>-0.61, 0.11</t>
   </si>
 </sst>
 </file>
@@ -733,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -772,6 +995,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9948B2D6-0D24-AC4F-B3C7-22D23935FFEB}">
   <dimension ref="A1:AN60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -10479,4 +10704,2026 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E0BD80-0BB3-E04A-A7FE-1D76F2CD0D51}">
+  <dimension ref="A1:Y37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="Y38" sqref="Y38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="38" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2437.06</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>1342.38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>2852.17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7">
+        <v>2151.67</v>
+      </c>
+      <c r="R7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7">
+        <v>149.09</v>
+      </c>
+      <c r="W7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3.15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.56</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="5">
+        <v>3.71</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y10" s="10"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0.66</v>
+      </c>
+      <c r="C11">
+        <v>0.81</v>
+      </c>
+      <c r="D11" s="6">
+        <v>49</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>0.03</v>
+      </c>
+      <c r="H11">
+        <v>0.17</v>
+      </c>
+      <c r="I11">
+        <v>44</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11">
+        <v>0.79</v>
+      </c>
+      <c r="M11">
+        <v>0.89</v>
+      </c>
+      <c r="N11" s="6">
+        <v>44</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11">
+        <v>0.13</v>
+      </c>
+      <c r="R11">
+        <v>0.35</v>
+      </c>
+      <c r="S11">
+        <v>61</v>
+      </c>
+      <c r="U11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11">
+        <v>0.03</v>
+      </c>
+      <c r="W11">
+        <v>0.16</v>
+      </c>
+      <c r="X11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>106</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>0.11</v>
+      </c>
+      <c r="H12">
+        <v>0.32</v>
+      </c>
+      <c r="I12">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>41</v>
+      </c>
+      <c r="P12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q12">
+        <v>0.05</v>
+      </c>
+      <c r="R12">
+        <v>0.23</v>
+      </c>
+      <c r="S12">
+        <v>45</v>
+      </c>
+      <c r="U12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>0.13</v>
+      </c>
+      <c r="C13">
+        <v>0.36</v>
+      </c>
+      <c r="D13">
+        <v>493</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>0.13</v>
+      </c>
+      <c r="H13">
+        <v>0.37</v>
+      </c>
+      <c r="I13">
+        <v>493</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13">
+        <v>0.27</v>
+      </c>
+      <c r="M13">
+        <v>0.52</v>
+      </c>
+      <c r="N13">
+        <v>483</v>
+      </c>
+      <c r="P13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13">
+        <v>0.15</v>
+      </c>
+      <c r="R13">
+        <v>0.38</v>
+      </c>
+      <c r="S13">
+        <v>684</v>
+      </c>
+      <c r="U13" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13">
+        <v>0.05</v>
+      </c>
+      <c r="W13">
+        <v>0.23</v>
+      </c>
+      <c r="X13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y15" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16">
+        <v>-0.24</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16">
+        <v>-1.36</v>
+      </c>
+      <c r="E16">
+        <v>0.18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G16">
+        <v>-0.23</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="I16">
+        <v>-0.81</v>
+      </c>
+      <c r="J16">
+        <v>0.42</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="N16" s="5">
+        <v>1.99</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="P16" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q16">
+        <v>-0.04</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="S16">
+        <v>-0.19</v>
+      </c>
+      <c r="T16">
+        <v>0.85</v>
+      </c>
+      <c r="U16" t="s">
+        <v>196</v>
+      </c>
+      <c r="V16">
+        <v>0.66</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="X16">
+        <v>1.2</v>
+      </c>
+      <c r="Y16">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17">
+        <v>-0.23</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17">
+        <v>-1.24</v>
+      </c>
+      <c r="E17">
+        <v>0.22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G17">
+        <v>-0.11</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I17">
+        <v>-0.43</v>
+      </c>
+      <c r="J17">
+        <v>0.67</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="N17" s="5">
+        <v>3.05</v>
+      </c>
+      <c r="O17" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="S17" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="T17" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="U17" t="s">
+        <v>197</v>
+      </c>
+      <c r="V17">
+        <v>0.8</v>
+      </c>
+      <c r="W17" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="X17">
+        <v>1.21</v>
+      </c>
+      <c r="Y17">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18">
+        <v>-0.3</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18">
+        <v>-1.82</v>
+      </c>
+      <c r="E18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>198</v>
+      </c>
+      <c r="G18">
+        <v>-0.22</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I18">
+        <v>-0.82</v>
+      </c>
+      <c r="J18">
+        <v>0.41</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="N18" s="5">
+        <v>3.35</v>
+      </c>
+      <c r="O18" s="5">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="P18" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S18" s="6">
+        <v>1.43</v>
+      </c>
+      <c r="T18" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="U18" t="s">
+        <v>198</v>
+      </c>
+      <c r="V18">
+        <v>0.78</v>
+      </c>
+      <c r="W18" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="X18">
+        <v>1.6</v>
+      </c>
+      <c r="Y18">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19">
+        <v>-0.03</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19">
+        <v>-0.16</v>
+      </c>
+      <c r="E19">
+        <v>0.88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19">
+        <v>-0.11</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="I19">
+        <v>-0.4</v>
+      </c>
+      <c r="J19">
+        <v>0.69</v>
+      </c>
+      <c r="K19" t="s">
+        <v>199</v>
+      </c>
+      <c r="L19">
+        <v>0.37</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="N19">
+        <v>1.74</v>
+      </c>
+      <c r="O19">
+        <v>0.08</v>
+      </c>
+      <c r="P19" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="S19" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="T19" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="V19" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="W19" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="X19" s="6">
+        <v>1.86</v>
+      </c>
+      <c r="Y19" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="23">
+        <v>-0.79</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="23">
+        <v>-3.04</v>
+      </c>
+      <c r="E20" s="23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="21">
+        <v>-0.47</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="I20" s="21">
+        <v>-1.64</v>
+      </c>
+      <c r="J20" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="L20" s="23">
+        <v>0.62</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" s="23">
+        <v>2.04</v>
+      </c>
+      <c r="O20" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="R20" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="S20" s="21">
+        <v>1.07</v>
+      </c>
+      <c r="T20" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="U20" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="V20" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="W20" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="X20" s="25">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="Y20" s="25">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="16" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="16">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0.27</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="L21" s="30">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="N21" s="30">
+        <v>-2.9</v>
+      </c>
+      <c r="O21" s="30">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>-0.03</v>
+      </c>
+      <c r="R21" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="S21" s="16">
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="T21" s="16">
+        <v>0.26</v>
+      </c>
+      <c r="U21" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="V21" s="16">
+        <v>-0.23</v>
+      </c>
+      <c r="W21" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="X21" s="16">
+        <v>-1.4</v>
+      </c>
+      <c r="Y21" s="16">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>3533.69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>915.15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <v>1522.54</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23">
+        <v>1041.78</v>
+      </c>
+      <c r="R23" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="W23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>1.03</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>0.95</v>
+      </c>
+      <c r="H24" t="s">
+        <v>201</v>
+      </c>
+      <c r="I24" t="s">
+        <v>194</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24">
+        <v>0.23</v>
+      </c>
+      <c r="R24" t="s">
+        <v>255</v>
+      </c>
+      <c r="S24" t="s">
+        <v>194</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24">
+        <v>1.41</v>
+      </c>
+      <c r="W24" t="s">
+        <v>195</v>
+      </c>
+      <c r="X24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O26" s="10"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T26" s="10"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y26" s="10"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>0.31</v>
+      </c>
+      <c r="C27">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D27" s="6">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>0.01</v>
+      </c>
+      <c r="H27">
+        <v>0.1</v>
+      </c>
+      <c r="I27">
+        <v>44</v>
+      </c>
+      <c r="K27" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27">
+        <v>0.03</v>
+      </c>
+      <c r="M27">
+        <v>0.18</v>
+      </c>
+      <c r="N27" s="6">
+        <v>44</v>
+      </c>
+      <c r="P27" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q27">
+        <v>0.03</v>
+      </c>
+      <c r="R27">
+        <v>0.18</v>
+      </c>
+      <c r="S27">
+        <v>61</v>
+      </c>
+      <c r="U27" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27">
+        <v>0.04</v>
+      </c>
+      <c r="W27">
+        <v>0.21</v>
+      </c>
+      <c r="X27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>106</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>41</v>
+      </c>
+      <c r="P28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28">
+        <v>0.05</v>
+      </c>
+      <c r="R28">
+        <v>0.23</v>
+      </c>
+      <c r="S28">
+        <v>45</v>
+      </c>
+      <c r="U28" t="s">
+        <v>45</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>10</v>
+      </c>
+      <c r="Y28" s="5"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>0.39</v>
+      </c>
+      <c r="C29">
+        <v>0.62</v>
+      </c>
+      <c r="D29">
+        <v>493</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29">
+        <v>0.08</v>
+      </c>
+      <c r="H29">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I29">
+        <v>493</v>
+      </c>
+      <c r="K29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29">
+        <v>0.09</v>
+      </c>
+      <c r="M29">
+        <v>0.3</v>
+      </c>
+      <c r="N29">
+        <v>483</v>
+      </c>
+      <c r="P29" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q29">
+        <v>0.03</v>
+      </c>
+      <c r="R29">
+        <v>0.18</v>
+      </c>
+      <c r="S29">
+        <v>684</v>
+      </c>
+      <c r="U29" t="s">
+        <v>17</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N31" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>12</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="T31" t="s">
+        <v>21</v>
+      </c>
+      <c r="V31" t="s">
+        <v>12</v>
+      </c>
+      <c r="W31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="X31" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" s="8">
+        <v>-0.03</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" s="8">
+        <v>-0.13</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="8">
+        <v>-0.01</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="I32" s="8">
+        <v>-0.05</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="L32" s="27">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="N32" s="27">
+        <v>-0.94</v>
+      </c>
+      <c r="O32" s="27">
+        <v>0.35</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R32" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="S32" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="T32" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="U32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="V32" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="W32" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="X32" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Y32" s="8">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="B33" s="25">
+        <v>-0.13</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" s="25">
+        <v>-0.61</v>
+      </c>
+      <c r="E33" s="25">
+        <v>0.54</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G33" s="21">
+        <v>-0.11</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="I33" s="21">
+        <v>-1.05</v>
+      </c>
+      <c r="J33" s="21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="L33" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="M33" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="N33" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="O33" s="25">
+        <v>0.93</v>
+      </c>
+      <c r="P33" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q33" s="25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R33" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="S33" s="25">
+        <v>0.79</v>
+      </c>
+      <c r="T33" s="25">
+        <v>0.43</v>
+      </c>
+      <c r="U33" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="V33" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="W33" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="X33" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="Y33" s="21">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34" s="25">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="25">
+        <v>-0.44</v>
+      </c>
+      <c r="E34" s="25">
+        <v>0.66</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="25">
+        <v>0</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="J34" s="25">
+        <v>0.99</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="L34" s="25">
+        <v>-0.03</v>
+      </c>
+      <c r="M34" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="N34" s="25">
+        <v>-0.43</v>
+      </c>
+      <c r="O34" s="25">
+        <v>0.67</v>
+      </c>
+      <c r="P34" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q34" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="R34" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="S34" s="25">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="T34" s="25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="U34" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="V34" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="W34" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="X34" s="25">
+        <v>1.51</v>
+      </c>
+      <c r="Y34" s="25">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="21">
+        <v>-0.32</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-1.82</v>
+      </c>
+      <c r="E35" s="21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="25">
+        <v>-0.01</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="I35" s="25">
+        <v>-0.13</v>
+      </c>
+      <c r="J35" s="25">
+        <v>0.89</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="L35" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="M35" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="N35" s="25">
+        <v>0.45</v>
+      </c>
+      <c r="O35" s="25">
+        <v>0.66</v>
+      </c>
+      <c r="P35" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q35" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="R35" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="S35" s="25">
+        <v>0.47</v>
+      </c>
+      <c r="T35" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="U35" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="V35" s="25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="W35" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="X35" s="25">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Y35" s="25">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="25">
+        <v>0.27</v>
+      </c>
+      <c r="E36" s="25">
+        <v>0.79</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="21">
+        <v>0.09</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="I36" s="21">
+        <v>0.72</v>
+      </c>
+      <c r="J36" s="21">
+        <v>0.47</v>
+      </c>
+      <c r="K36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="L36" s="25">
+        <v>0.22</v>
+      </c>
+      <c r="M36" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="N36" s="25">
+        <v>1.32</v>
+      </c>
+      <c r="O36" s="25">
+        <v>0.19</v>
+      </c>
+      <c r="P36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q36" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="R36" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="S36" s="25">
+        <v>0.54</v>
+      </c>
+      <c r="T36" s="25">
+        <v>0.59</v>
+      </c>
+      <c r="U36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="V36" s="25">
+        <v>0.47</v>
+      </c>
+      <c r="W36" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="X36" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="Y36" s="25">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" s="16" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" s="16">
+        <v>0.53</v>
+      </c>
+      <c r="E37" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G37" s="16">
+        <v>-0.01</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="I37" s="16">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="J37" s="16">
+        <v>0.78</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="L37" s="16">
+        <v>0</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="N37" s="16">
+        <v>0.16</v>
+      </c>
+      <c r="O37" s="16">
+        <v>0.87</v>
+      </c>
+      <c r="P37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q37" s="16">
+        <v>-0.01</v>
+      </c>
+      <c r="R37" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="S37" s="16">
+        <v>-0.4</v>
+      </c>
+      <c r="T37" s="16">
+        <v>0.69</v>
+      </c>
+      <c r="U37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="V37" s="16">
+        <v>-0.25</v>
+      </c>
+      <c r="W37" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="X37" s="16">
+        <v>-1.36</v>
+      </c>
+      <c r="Y37" s="16">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>